<commit_message>
new icons + banner homeScreen + aiSetup made
</commit_message>
<xml_diff>
--- a/Stratego/resources/other/Pawn Powers.xlsx
+++ b/Stratego/resources/other/Pawn Powers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toon\Desktop\java Stratego\Stratego\resources\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8877FDB-516F-4208-B6CE-4A20CB346D5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CAC6FC-C3E6-4D54-8FEB-A2F4FFE511C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{589F3506-2B18-443E-8B1A-D64BB8D3ED99}"/>
   </bookViews>
@@ -137,17 +137,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55BCF6CF-2F2E-4F50-B20A-E30739F760F2}" name="Table1" displayName="Table1" ref="A1:D21" totalsRowShown="0">
-  <autoFilter ref="A1:D21" xr:uid="{3B33EC23-6CF7-4980-B2BD-6451CE30B1FE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55BCF6CF-2F2E-4F50-B20A-E30739F760F2}" name="Table1" displayName="Table1" ref="A1:D13" totalsRowShown="0">
+  <autoFilter ref="A1:D13" xr:uid="{3B33EC23-6CF7-4980-B2BD-6451CE30B1FE}"/>
   <tableColumns count="4">
+    <tableColumn id="2" xr3:uid="{0A08FC39-EF71-4ADC-958E-E4F497D4BE34}" name="RankType"/>
     <tableColumn id="1" xr3:uid="{9D4EA3E6-D7EC-4D59-9BD3-D586F2ED049B}" name="Count"/>
-    <tableColumn id="2" xr3:uid="{0A08FC39-EF71-4ADC-958E-E4F497D4BE34}" name="RankType"/>
     <tableColumn id="3" xr3:uid="{56EFDF26-2EE0-484B-A841-ECA2770B3751}" name="Power"/>
     <tableColumn id="4" xr3:uid="{460BA996-138C-4FBF-A11A-52B0261A204D}" name="Column1" dataDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[Power]]*Table1[[#This Row],[Count]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748C996E-3BDD-4D07-A77F-CFFDC152521F}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,10 +463,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -476,11 +476,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -491,11 +491,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
       <c r="C3">
         <v>90</v>
@@ -506,11 +506,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
         <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
       </c>
       <c r="C4">
         <v>80</v>
@@ -521,11 +521,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
         <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -536,11 +536,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
         <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
       </c>
       <c r="C6">
         <v>60</v>
@@ -551,11 +551,11 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
         <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
       </c>
       <c r="C7">
         <v>50</v>
@@ -566,11 +566,11 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
         <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
       </c>
       <c r="C8">
         <v>40</v>
@@ -581,11 +581,11 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
         <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -596,11 +596,11 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
         <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
       </c>
       <c r="C10">
         <v>30</v>
@@ -611,11 +611,11 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
         <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
       </c>
       <c r="C11">
         <v>70</v>
@@ -626,11 +626,11 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
         <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
       </c>
       <c r="C12">
         <v>40</v>
@@ -641,13 +641,9 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f>SUBTOTAL(109,A2:A12)</f>
-        <v>40</v>
-      </c>
       <c r="B13">
         <f>SUBTOTAL(109,B2:B12)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <f>SUBTOTAL(109,D2:D12)</f>

</xml_diff>